<commit_message>
bidirectional synapses, update to work with my new superneuromat
</commit_message>
<xml_diff>
--- a/cora.xlsx
+++ b/cora.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b57a024f052910e/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b57a024f052910e/Documents/.projects/blimplab/neuromorphic/superneuro/sgnn-superneuro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{33AB184F-2F2F-41A7-9F30-E0A8D5E56D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37F7ED9E-AF3A-40CF-8ACB-1BB648BE363E}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{33AB184F-2F2F-41A7-9F30-E0A8D5E56D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05C631F9-DFB3-4AF3-94BE-5CD9BAA4DCFD}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{307C9579-482A-4687-9092-340442B884B1}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{307C9579-482A-4687-9092-340442B884B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
   <si>
     <t>perfect</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>evaluation spikes</t>
+  </si>
+  <si>
+    <t>bidirectional</t>
   </si>
 </sst>
 </file>
@@ -534,27 +537,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB7C963E-B532-4144-91BF-372CEDAB96A0}">
-  <dimension ref="A1:O71"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="P69" sqref="P69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q73" sqref="Q73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.765625" customWidth="1"/>
-    <col min="2" max="5" width="4.765625" customWidth="1"/>
-    <col min="6" max="6" width="9.23046875" customWidth="1"/>
-    <col min="7" max="7" width="5.765625" customWidth="1"/>
-    <col min="8" max="8" width="16.84375" customWidth="1"/>
+    <col min="1" max="1" width="5.77734375" customWidth="1"/>
+    <col min="2" max="5" width="4.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" customWidth="1"/>
+    <col min="7" max="7" width="5.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="14.84375" customWidth="1"/>
-    <col min="11" max="11" width="14.53515625" customWidth="1"/>
-    <col min="12" max="12" width="8.4609375" customWidth="1"/>
-    <col min="13" max="13" width="12.3046875" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" customWidth="1"/>
+    <col min="12" max="12" width="8.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,10 +605,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>219</v>
       </c>
@@ -651,7 +655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>219</v>
       </c>
@@ -698,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>109</v>
       </c>
@@ -745,7 +749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>72</v>
       </c>
@@ -792,7 +796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>17</v>
       </c>
@@ -839,7 +843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>219</v>
       </c>
@@ -886,7 +890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>219</v>
       </c>
@@ -933,7 +937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>177</v>
       </c>
@@ -980,7 +984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>81</v>
       </c>
@@ -1027,7 +1031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>219</v>
       </c>
@@ -1074,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>219</v>
       </c>
@@ -1121,7 +1125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>219</v>
       </c>
@@ -1168,7 +1172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>219</v>
       </c>
@@ -1215,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>177</v>
       </c>
@@ -1262,7 +1266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>81</v>
       </c>
@@ -1309,7 +1313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>219</v>
       </c>
@@ -1356,7 +1360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>177</v>
       </c>
@@ -1403,7 +1407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>81</v>
       </c>
@@ -1450,7 +1454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>80</v>
       </c>
@@ -1497,7 +1501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1544,7 +1548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -1591,7 +1595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>83</v>
       </c>
@@ -1638,7 +1642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>212</v>
       </c>
@@ -1685,7 +1689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>219</v>
       </c>
@@ -1732,7 +1736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>100</v>
       </c>
@@ -1779,7 +1783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>72</v>
       </c>
@@ -1826,7 +1830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1873,12 +1877,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="O36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>219</v>
       </c>
@@ -1925,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>219</v>
       </c>
@@ -1972,7 +1976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>219</v>
       </c>
@@ -2019,7 +2023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>219</v>
       </c>
@@ -2066,7 +2070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>219</v>
       </c>
@@ -2113,7 +2117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>219</v>
       </c>
@@ -2160,7 +2164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>219</v>
       </c>
@@ -2207,7 +2211,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>219</v>
       </c>
@@ -2254,7 +2258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>219</v>
       </c>
@@ -2301,7 +2305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>219</v>
       </c>
@@ -2348,7 +2352,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>219</v>
       </c>
@@ -2395,7 +2399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>219</v>
       </c>
@@ -2442,7 +2446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>219</v>
       </c>
@@ -2489,7 +2493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>219</v>
       </c>
@@ -2536,7 +2540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>219</v>
       </c>
@@ -2583,7 +2587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>219</v>
       </c>
@@ -2630,7 +2634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>219</v>
       </c>
@@ -2677,7 +2681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>219</v>
       </c>
@@ -2724,7 +2728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>219</v>
       </c>
@@ -2771,7 +2775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>219</v>
       </c>
@@ -2818,7 +2822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>219</v>
       </c>
@@ -2865,7 +2869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>219</v>
       </c>
@@ -2912,7 +2916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>219</v>
       </c>
@@ -2959,7 +2963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>219</v>
       </c>
@@ -3006,7 +3010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>219</v>
       </c>
@@ -3053,7 +3057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>205</v>
       </c>
@@ -3100,7 +3104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>219</v>
       </c>
@@ -3147,7 +3151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>219</v>
       </c>
@@ -3194,7 +3198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>178</v>
       </c>
@@ -3241,7 +3245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>179</v>
       </c>
@@ -3288,7 +3292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>0</v>
       </c>
@@ -3335,7 +3339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>219</v>
       </c>
@@ -3382,7 +3386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>219</v>
       </c>
@@ -3427,6 +3431,100 @@
       </c>
       <c r="O71">
         <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>318</v>
+      </c>
+      <c r="B72">
+        <v>396</v>
+      </c>
+      <c r="C72">
+        <v>137</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>115</v>
+      </c>
+      <c r="F72">
+        <v>426</v>
+      </c>
+      <c r="G72">
+        <v>541</v>
+      </c>
+      <c r="H72" t="s">
+        <v>22</v>
+      </c>
+      <c r="I72" t="s">
+        <v>21</v>
+      </c>
+      <c r="J72">
+        <v>2</v>
+      </c>
+      <c r="K72">
+        <v>5</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="M72" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="N72">
+        <v>5.9</v>
+      </c>
+      <c r="P72" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>361</v>
+      </c>
+      <c r="B73">
+        <v>490</v>
+      </c>
+      <c r="C73">
+        <v>230</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>17</v>
+      </c>
+      <c r="F73">
+        <v>524</v>
+      </c>
+      <c r="G73">
+        <v>541</v>
+      </c>
+      <c r="H73" t="s">
+        <v>22</v>
+      </c>
+      <c r="I73" t="s">
+        <v>21</v>
+      </c>
+      <c r="J73">
+        <v>2</v>
+      </c>
+      <c r="K73">
+        <v>5</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="M73" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="N73">
+        <v>4.3319999999999999</v>
+      </c>
+      <c r="P73" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>